<commit_message>
:recycle: refactor: acc alumni
</commit_message>
<xml_diff>
--- a/public/tracer-study-linearitas.xlsx
+++ b/public/tracer-study-linearitas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Putra\Kuliah\S6\PENGSI\tracer-study\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E7348AC-4DA2-4644-95B9-DA911F7D09D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1C7E5D1-FFC0-4CA9-9E9D-4A64E5187761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" xr2:uid="{994F8ED6-DB87-4DD1-B5AD-053B2AD6140F}"/>
   </bookViews>
@@ -509,8 +509,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93FF527-C178-47E1-8E72-5B62F92DA900}">
   <dimension ref="A1:F359"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A187" workbookViewId="0">
-      <selection activeCell="F197" sqref="F197:F359"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>